<commit_message>
fix bug không vào được chức năng sửa
</commit_message>
<xml_diff>
--- a/QuanLyNhanSuApp/quanlynhansu.xlsx
+++ b/QuanLyNhanSuApp/quanlynhansu.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\LTUD\Project\cuoiki\QuanLyNhanSu\QuanLyNhanSuApp\"/>
     </mc:Choice>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="114">
   <si>
     <t>maPhong</t>
   </si>
@@ -282,6 +282,87 @@
   </si>
   <si>
     <t>cntt@company.com</t>
+  </si>
+  <si>
+    <t>1998-05-12</t>
+  </si>
+  <si>
+    <t>79198001234</t>
+  </si>
+  <si>
+    <t>2000-03-20</t>
+  </si>
+  <si>
+    <t>79200123456</t>
+  </si>
+  <si>
+    <t>1997-11-10</t>
+  </si>
+  <si>
+    <t>79197654321</t>
+  </si>
+  <si>
+    <t>1999-09-25</t>
+  </si>
+  <si>
+    <t>79199789123</t>
+  </si>
+  <si>
+    <t>1995-01-17</t>
+  </si>
+  <si>
+    <t>79195456987</t>
+  </si>
+  <si>
+    <t>2001-07-02</t>
+  </si>
+  <si>
+    <t>79201987654</t>
+  </si>
+  <si>
+    <t>1996-12-08</t>
+  </si>
+  <si>
+    <t>79196321789</t>
+  </si>
+  <si>
+    <t>1998-08-30</t>
+  </si>
+  <si>
+    <t>79198951753</t>
+  </si>
+  <si>
+    <t>1994-04-15</t>
+  </si>
+  <si>
+    <t>79194753951</t>
+  </si>
+  <si>
+    <t>2000-10-05</t>
+  </si>
+  <si>
+    <t>79200852369</t>
+  </si>
+  <si>
+    <t>NV011</t>
+  </si>
+  <si>
+    <t>La Gia Lộc</t>
+  </si>
+  <si>
+    <t>2004-03-02</t>
+  </si>
+  <si>
+    <t>0982482424</t>
+  </si>
+  <si>
+    <t>locla.323232@gmail.com</t>
+  </si>
+  <si>
+    <t>0923882498</t>
+  </si>
+  <si>
+    <t>Phó phòng</t>
   </si>
 </sst>
 </file>
@@ -646,132 +727,132 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.28515625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.140625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.5703125"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="12.85546875"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="25.0"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2">
+      <c r="A2" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>72</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s" s="1">
         <v>73</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>74</v>
       </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="F2" t="n" s="0">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>75</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s" s="1">
         <v>76</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>77</v>
       </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="F3" t="n" s="0">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>78</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>31</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s" s="1">
         <v>79</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>80</v>
       </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="F4" t="n" s="0">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>81</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s" s="1">
         <v>82</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>83</v>
       </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="F5" t="n" s="0">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>84</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s" s="1">
         <v>85</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>86</v>
       </c>
-      <c r="F6">
-        <v>2</v>
+      <c r="F6" t="n" s="0">
+        <v>2.0</v>
       </c>
     </row>
   </sheetData>
@@ -781,7 +862,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
@@ -789,25 +870,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.7109375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.140625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.140625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="10.42578125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="12.0"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="26.140625"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.0"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.5703125"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="24.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -816,307 +897,336 @@
       <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2">
+      <c r="A2" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="D2" s="2">
-        <v>35927</v>
-      </c>
-      <c r="E2" s="1">
-        <v>79198001234</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="D2" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="E2" t="s" s="1">
+        <v>88</v>
+      </c>
+      <c r="F2" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" t="s" s="1">
         <v>62</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3">
+      <c r="A3" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="D3" s="2">
-        <v>36605</v>
-      </c>
-      <c r="E3" s="1">
-        <v>79200123456</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="D3" t="s" s="2">
+        <v>89</v>
+      </c>
+      <c r="E3" t="s" s="1">
+        <v>90</v>
+      </c>
+      <c r="F3" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" t="s" s="1">
         <v>63</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4">
+      <c r="A4" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="D4" s="2">
-        <v>35744</v>
-      </c>
-      <c r="E4" s="1">
-        <v>79197654321</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="D4" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="E4" t="s" s="1">
+        <v>92</v>
+      </c>
+      <c r="F4" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" t="s" s="1">
         <v>64</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" t="s" s="0">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5">
+      <c r="A5" t="s" s="0">
         <v>31</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="D5" s="2">
-        <v>36428</v>
-      </c>
-      <c r="E5" s="1">
-        <v>79199789123</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="D5" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="E5" t="s" s="1">
+        <v>94</v>
+      </c>
+      <c r="F5" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" t="s" s="1">
         <v>65</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" t="s" s="0">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6">
+      <c r="A6" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="D6" s="2">
-        <v>34716</v>
-      </c>
-      <c r="E6" s="1">
-        <v>79195456987</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="D6" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="E6" t="s" s="1">
+        <v>96</v>
+      </c>
+      <c r="F6" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" t="s" s="1">
         <v>66</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" t="s" s="0">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7">
+      <c r="A7" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="D7" s="2">
-        <v>37074</v>
-      </c>
-      <c r="E7" s="1">
-        <v>79201987654</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="D7" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="E7" t="s" s="1">
+        <v>98</v>
+      </c>
+      <c r="F7" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" t="s" s="1">
         <v>67</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" t="s" s="0">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8">
+      <c r="A8" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="D8" s="2">
-        <v>35407</v>
-      </c>
-      <c r="E8" s="1">
-        <v>79196321789</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="D8" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="E8" t="s" s="1">
+        <v>100</v>
+      </c>
+      <c r="F8" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" t="s" s="1">
         <v>68</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" t="s" s="0">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9">
+      <c r="A9" t="s" s="0">
         <v>50</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="D9" s="2">
-        <v>36037</v>
-      </c>
-      <c r="E9" s="1">
-        <v>79198951753</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="D9" t="s" s="2">
+        <v>101</v>
+      </c>
+      <c r="E9" t="s" s="1">
+        <v>102</v>
+      </c>
+      <c r="F9" t="s" s="0">
         <v>52</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" t="s" s="1">
         <v>69</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" t="s" s="0">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10">
+      <c r="A10" t="s" s="0">
         <v>54</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="D10" s="2">
-        <v>34439</v>
-      </c>
-      <c r="E10" s="1">
-        <v>79194753951</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="D10" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="E10" t="s" s="1">
+        <v>104</v>
+      </c>
+      <c r="F10" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" t="s" s="1">
         <v>70</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" t="s" s="0">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11">
+      <c r="A11" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="D11" s="2">
-        <v>36804</v>
-      </c>
-      <c r="E11" s="1">
-        <v>79200852369</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="D11" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="E11" t="s" s="1">
+        <v>106</v>
+      </c>
+      <c r="F11" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" t="s" s="1">
         <v>71</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" t="s" s="0">
         <v>61</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>107</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>108</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s" s="2">
+        <v>109</v>
+      </c>
+      <c r="E12" t="s" s="1">
+        <v>110</v>
+      </c>
+      <c r="F12" t="s" s="0">
+        <v>111</v>
+      </c>
+      <c r="G12" t="s" s="1">
+        <v>112</v>
+      </c>
+      <c r="H12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="I12" t="s" s="0">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
thêm chức năng quay lại giao diện chính (lựa chọn nhân sự / phòng ban)
</commit_message>
<xml_diff>
--- a/QuanLyNhanSuApp/quanlynhansu.xlsx
+++ b/QuanLyNhanSuApp/quanlynhansu.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="115">
   <si>
     <t>maPhong</t>
   </si>
@@ -363,6 +363,9 @@
   </si>
   <si>
     <t>Phó phòng</t>
+  </si>
+  <si>
+    <t>P00</t>
   </si>
 </sst>
 </file>
@@ -719,7 +722,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D1" sqref="A1:XFD1048576"/>
@@ -772,44 +775,44 @@
         <v>74</v>
       </c>
       <c r="F2" t="n" s="0">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s" s="1">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F3" t="n" s="0">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s" s="1">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F4" t="n" s="0">
         <v>2.0</v>
@@ -817,42 +820,22 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s" s="1">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F5" t="n" s="0">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
-        <v>48</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>84</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="D6" t="s" s="1">
-        <v>85</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>86</v>
-      </c>
-      <c r="F6" t="n" s="0">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
   </sheetData>
@@ -962,7 +945,7 @@
         <v>63</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="I3" t="s" s="0">
         <v>26</v>
@@ -1078,7 +1061,7 @@
         <v>67</v>
       </c>
       <c r="H7" t="s" s="0">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="I7" t="s" s="0">
         <v>44</v>
@@ -1223,7 +1206,7 @@
         <v>112</v>
       </c>
       <c r="H12" t="s" s="0">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="I12" t="s" s="0">
         <v>113</v>

</xml_diff>

<commit_message>
chỉnh thông báo xóa
</commit_message>
<xml_diff>
--- a/QuanLyNhanSuApp/quanlynhansu.xlsx
+++ b/QuanLyNhanSuApp/quanlynhansu.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="115">
   <si>
     <t>maPhong</t>
   </si>
@@ -363,6 +363,9 @@
   </si>
   <si>
     <t>Phó phòng</t>
+  </si>
+  <si>
+    <t>Phạm Thị Bông Hồng</t>
   </si>
 </sst>
 </file>
@@ -1002,7 +1005,7 @@
         <v>31</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>32</v>
+        <v>114</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>23</v>

</xml_diff>

<commit_message>
giải quyết các vấn đề từ 1 - 11
</commit_message>
<xml_diff>
--- a/QuanLyNhanSuApp/quanlynhansu.xlsx
+++ b/QuanLyNhanSuApp/quanlynhansu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\LTUD\Project\cuoiki\QuanLyNhanSu\QuanLyNhanSuApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2470FDCB-EBA0-4F3A-B866-4202642B518D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C8819A-88B6-4303-BEA5-951B0C931C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="4185" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PhongBan" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="110">
   <si>
     <t>maPhong</t>
   </si>
@@ -98,9 +98,6 @@
     <t>bich.tran@company.com</t>
   </si>
   <si>
-    <t>PB02</t>
-  </si>
-  <si>
     <t>Nhân viên Kế toán</t>
   </si>
   <si>
@@ -248,15 +245,6 @@
     <t>kinhdoanh@company.com</t>
   </si>
   <si>
-    <t>Phòng Kế toán</t>
-  </si>
-  <si>
-    <t>028 3567 2234</t>
-  </si>
-  <si>
-    <t>ketoan@company.com</t>
-  </si>
-  <si>
     <t>Phòng Hành chính</t>
   </si>
   <si>
@@ -284,88 +272,85 @@
     <t>cntt@company.com</t>
   </si>
   <si>
+    <t>NV011</t>
+  </si>
+  <si>
+    <t>La Gia Lộc</t>
+  </si>
+  <si>
+    <t>0982482424</t>
+  </si>
+  <si>
+    <t>locla.323232@gmail.com</t>
+  </si>
+  <si>
+    <t>0923882498</t>
+  </si>
+  <si>
+    <t>Phó phòng</t>
+  </si>
+  <si>
+    <t>079198001234</t>
+  </si>
+  <si>
+    <t>079200123456</t>
+  </si>
+  <si>
+    <t>079199789123</t>
+  </si>
+  <si>
+    <t>079197654321</t>
+  </si>
+  <si>
+    <t>079195456987</t>
+  </si>
+  <si>
+    <t>079201987654</t>
+  </si>
+  <si>
+    <t>079196321789</t>
+  </si>
+  <si>
+    <t>079198951753</t>
+  </si>
+  <si>
+    <t>079194753951</t>
+  </si>
+  <si>
+    <t>079200852369</t>
+  </si>
+  <si>
     <t>1998-05-12</t>
   </si>
   <si>
-    <t>79198001234</t>
-  </si>
-  <si>
     <t>2000-03-20</t>
   </si>
   <si>
-    <t>79200123456</t>
-  </si>
-  <si>
     <t>1997-11-10</t>
   </si>
   <si>
-    <t>79197654321</t>
-  </si>
-  <si>
     <t>1999-09-25</t>
   </si>
   <si>
-    <t>79199789123</t>
-  </si>
-  <si>
     <t>1995-01-17</t>
   </si>
   <si>
-    <t>79195456987</t>
-  </si>
-  <si>
     <t>2001-07-02</t>
   </si>
   <si>
-    <t>79201987654</t>
-  </si>
-  <si>
     <t>1996-12-08</t>
   </si>
   <si>
-    <t>79196321789</t>
-  </si>
-  <si>
     <t>1998-08-30</t>
   </si>
   <si>
-    <t>79198951753</t>
-  </si>
-  <si>
     <t>1994-04-15</t>
   </si>
   <si>
-    <t>79194753951</t>
-  </si>
-  <si>
     <t>2000-10-05</t>
   </si>
   <si>
-    <t>79200852369</t>
-  </si>
-  <si>
-    <t>NV011</t>
-  </si>
-  <si>
-    <t>La Gia Lộc</t>
-  </si>
-  <si>
-    <t>2004-03-02</t>
-  </si>
-  <si>
-    <t>0982482424</t>
-  </si>
-  <si>
-    <t>locla.323232@gmail.com</t>
-  </si>
-  <si>
-    <t>0923882498</t>
-  </si>
-  <si>
-    <t>Phó phòng</t>
-  </si>
-  <si>
-    <t>P00</t>
+    <t>2003-03-02</t>
   </si>
 </sst>
 </file>
@@ -373,7 +358,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -404,10 +389,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -724,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,16 +749,16 @@
         <v>19</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s" s="0">
         <v>15</v>
       </c>
       <c r="D2" t="s" s="1">
+        <v>72</v>
+      </c>
+      <c r="E2" t="s" s="0">
         <v>73</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>74</v>
       </c>
       <c r="F2" t="n" s="0">
         <v>3.0</v>
@@ -780,19 +766,19 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s" s="1">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F3" t="n" s="0">
         <v>2.0</v>
@@ -800,19 +786,19 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s" s="1">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F4" t="n" s="0">
         <v>2.0</v>
@@ -820,19 +806,19 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s" s="1">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F5" t="n" s="0">
         <v>4.0</v>
@@ -847,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,12 +842,13 @@
     <col min="1" max="1" bestFit="true" customWidth="true" width="6.7109375"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="15.140625"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="8.140625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="10.42578125"/>
+    <col min="4" max="4" customWidth="true" style="2" width="14.28515625"/>
     <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="12.0"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="26.140625"/>
     <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="11.0"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="12.5703125"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="24.28515625"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="3" width="10.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -904,16 +891,16 @@
         <v>17</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="E2" t="s" s="1">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F2" t="s" s="0">
         <v>18</v>
       </c>
       <c r="G2" t="s" s="1">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H2" t="s" s="0">
         <v>19</v>
@@ -933,7 +920,7 @@
         <v>23</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="E3" t="s" s="1">
         <v>90</v>
@@ -942,253 +929,253 @@
         <v>24</v>
       </c>
       <c r="G3" t="s" s="1">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H3" t="s" s="0">
         <v>19</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s" s="0">
         <v>27</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>28</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>17</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="E4" t="s" s="1">
         <v>92</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G4" t="s" s="1">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H4" t="s" s="0">
         <v>19</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s" s="0">
         <v>31</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>32</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>23</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E5" t="s" s="1">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F5" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="G5" t="s" s="1">
+        <v>64</v>
+      </c>
+      <c r="H5" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="G5" t="s" s="1">
-        <v>65</v>
-      </c>
-      <c r="H5" t="s" s="0">
+      <c r="I5" t="s" s="0">
         <v>34</v>
-      </c>
-      <c r="I5" t="s" s="0">
-        <v>35</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s" s="0">
         <v>36</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>37</v>
       </c>
       <c r="C6" t="s" s="0">
         <v>17</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="E6" t="s" s="1">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F6" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="G6" t="s" s="1">
+        <v>65</v>
+      </c>
+      <c r="H6" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="G6" t="s" s="1">
-        <v>66</v>
-      </c>
-      <c r="H6" t="s" s="0">
+      <c r="I6" t="s" s="0">
         <v>39</v>
-      </c>
-      <c r="I6" t="s" s="0">
-        <v>40</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s" s="0">
         <v>41</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>42</v>
       </c>
       <c r="C7" t="s" s="0">
         <v>23</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="E7" t="s" s="1">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F7" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="G7" t="s" s="1">
+        <v>66</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="I7" t="s" s="0">
         <v>43</v>
-      </c>
-      <c r="G7" t="s" s="1">
-        <v>67</v>
-      </c>
-      <c r="H7" t="s" s="0">
-        <v>48</v>
-      </c>
-      <c r="I7" t="s" s="0">
-        <v>44</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="B8" t="s" s="0">
         <v>45</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>46</v>
       </c>
       <c r="C8" t="s" s="0">
         <v>17</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="E8" t="s" s="1">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F8" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="G8" t="s" s="1">
+        <v>67</v>
+      </c>
+      <c r="H8" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="G8" t="s" s="1">
-        <v>68</v>
-      </c>
-      <c r="H8" t="s" s="0">
+      <c r="I8" t="s" s="0">
         <v>48</v>
-      </c>
-      <c r="I8" t="s" s="0">
-        <v>49</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s" s="0">
         <v>50</v>
-      </c>
-      <c r="B9" t="s" s="0">
-        <v>51</v>
       </c>
       <c r="C9" t="s" s="0">
         <v>23</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E9" t="s" s="1">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F9" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="G9" t="s" s="1">
+        <v>68</v>
+      </c>
+      <c r="H9" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="I9" t="s" s="0">
         <v>52</v>
-      </c>
-      <c r="G9" t="s" s="1">
-        <v>69</v>
-      </c>
-      <c r="H9" t="s" s="0">
-        <v>48</v>
-      </c>
-      <c r="I9" t="s" s="0">
-        <v>53</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s" s="0">
         <v>54</v>
-      </c>
-      <c r="B10" t="s" s="0">
-        <v>55</v>
       </c>
       <c r="C10" t="s" s="0">
         <v>17</v>
       </c>
       <c r="D10" t="s" s="2">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="E10" t="s" s="1">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="F10" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="G10" t="s" s="1">
+        <v>69</v>
+      </c>
+      <c r="H10" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="I10" t="s" s="0">
         <v>56</v>
-      </c>
-      <c r="G10" t="s" s="1">
-        <v>70</v>
-      </c>
-      <c r="H10" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="I10" t="s" s="0">
-        <v>57</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="B11" t="s" s="0">
         <v>58</v>
-      </c>
-      <c r="B11" t="s" s="0">
-        <v>59</v>
       </c>
       <c r="C11" t="s" s="0">
         <v>23</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E11" t="s" s="1">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F11" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="G11" t="s" s="1">
+        <v>70</v>
+      </c>
+      <c r="H11" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="I11" t="s" s="0">
         <v>60</v>
-      </c>
-      <c r="G11" t="s" s="1">
-        <v>71</v>
-      </c>
-      <c r="H11" t="s" s="0">
-        <v>39</v>
-      </c>
-      <c r="I11" t="s" s="0">
-        <v>61</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="C12" t="s" s="0">
         <v>17</v>
@@ -1197,22 +1184,23 @@
         <v>109</v>
       </c>
       <c r="E12" t="s" s="1">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="F12" t="s" s="0">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="G12" t="s" s="1">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="H12" t="s" s="0">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I12" t="s" s="0">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>